<commit_message>
feat: Office viewer 的 Excel 中实现公式解析和执行
</commit_message>
<xml_diff>
--- a/packages/office-viewer/__tests__/xlsx/simple/definedName.xlsx
+++ b/packages/office-viewer/__tests__/xlsx/simple/definedName.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nwind/working/icode/amis/amis/amis-office/packages/office-viewer/__tests__/xlsx/simple/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B95B277-87AB-6E4B-95D0-9123960B24B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F5364E-1C81-7E43-89C3-AE71EC223316}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8920" yWindow="4600" windowWidth="26840" windowHeight="15940" xr2:uid="{B23FB826-BDED-B44E-9790-D097C5C49E7D}"/>
   </bookViews>
@@ -18,6 +18,7 @@
   <definedNames>
     <definedName name="name1">Sheet1!$B$2:$B$6</definedName>
     <definedName name="name2">Sheet1!$D$3:$H$3</definedName>
+    <definedName name="name3">Sheet1!$D$2:$D$5,Sheet1!$G$2:$G$6</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -409,7 +410,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>